<commit_message>
feat: update test case
</commit_message>
<xml_diff>
--- a/Testcase.xlsx
+++ b/Testcase.xlsx
@@ -1,13 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\education-group-project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3C1A1E-418A-4407-A460-D726589661F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="registerlogin" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="CRUD Courses" sheetId="2" r:id="rId5"/>
+    <sheet name="registerlogin" sheetId="1" r:id="rId1"/>
+    <sheet name="CRUD Courses" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -256,13 +265,14 @@
   </si>
   <si>
     <r>
-      <rPr/>
       <t xml:space="preserve">1. Nhập </t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t>abcgmail.com</t>
     </r>
@@ -1776,28 +1786,37 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1805,7 +1824,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1839,67 +1858,59 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -2089,29 +2100,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="22.38"/>
-    <col customWidth="1" min="3" max="3" width="19.63"/>
-    <col customWidth="1" min="4" max="4" width="19.5"/>
-    <col customWidth="1" min="5" max="5" width="26.63"/>
-    <col customWidth="1" min="6" max="6" width="26.13"/>
-    <col customWidth="1" min="7" max="7" width="25.5"/>
-    <col customWidth="1" min="9" max="9" width="35.63"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2140,36 +2156,48 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -2179,77 +2207,83 @@
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -2258,32 +2292,32 @@
       <c r="E11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -2296,11 +2330,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -2313,11 +2347,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -2330,7 +2364,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>55</v>
       </c>
@@ -2340,18 +2374,18 @@
       <c r="D16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -2364,28 +2398,28 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -2398,11 +2432,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>76</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -2415,11 +2449,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -2432,11 +2466,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -2449,28 +2483,28 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>91</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -2483,7 +2517,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>96</v>
       </c>
@@ -2500,7 +2534,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>101</v>
       </c>
@@ -2510,137 +2544,137 @@
       <c r="D26" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="5" t="s">
         <v>104</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>112</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>117</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="5" t="s">
         <v>122</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>127</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="5" t="s">
         <v>132</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="5" t="s">
         <v>139</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>142</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -2649,15 +2683,15 @@
       <c r="E34" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="5" t="s">
         <v>147</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -2666,15 +2700,15 @@
       <c r="E35" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>151</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -2687,11 +2721,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="5" t="s">
         <v>156</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -2700,15 +2734,15 @@
       <c r="E37" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="5" t="s">
         <v>160</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -2717,15 +2751,15 @@
       <c r="E38" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="5" t="s">
         <v>164</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -2734,18 +2768,18 @@
       <c r="E39" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>167</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="7" t="s">
         <v>169</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -2755,7 +2789,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>172</v>
       </c>
@@ -2772,7 +2806,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>174</v>
       </c>
@@ -2785,11 +2819,11 @@
       <c r="E42" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>179</v>
       </c>
@@ -2802,15 +2836,15 @@
       <c r="E43" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F43" s="5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5" t="s">
         <v>184</v>
       </c>
       <c r="D44" s="3" t="s">
@@ -2823,75 +2857,75 @@
         <v>187</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="7" t="s">
         <v>190</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="7" t="s">
         <v>195</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F46" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="7" t="s">
         <v>200</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>203</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="5" t="s">
         <v>206</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>207</v>
       </c>
@@ -2908,48 +2942,54 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>209</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="5" t="s">
         <v>213</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="9" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="52">
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="5" t="s">
         <v>217</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="F52" s="5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>220</v>
       </c>
@@ -2960,11 +3000,11 @@
       <c r="E53" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F53" s="5" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>224</v>
       </c>
@@ -2974,20 +3014,26 @@
       <c r="E54" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F54" s="5" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="9" t="s">
         <v>228</v>
       </c>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
       <c r="I55" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>230</v>
       </c>
@@ -3001,7 +3047,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>234</v>
       </c>
@@ -3015,11 +3061,11 @@
         <v>237</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="5" t="s">
         <v>239</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -3029,7 +3075,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>242</v>
       </c>
@@ -3039,11 +3085,11 @@
       <c r="E59" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="F59" s="5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>246</v>
       </c>
@@ -3057,7 +3103,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>250</v>
       </c>
@@ -3067,112 +3113,124 @@
       <c r="E61" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="F61" s="8" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="6"/>
-      <c r="B62" s="5" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="9" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="63">
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="5" t="s">
         <v>257</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="F63" s="5" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="5" t="s">
         <v>262</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="5" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>265</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="5" t="s">
         <v>267</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="5" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>269</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="5" t="s">
         <v>271</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="F66" s="7" t="s">
+      <c r="F66" s="5" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="6"/>
-      <c r="B67" s="5" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="9" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="68">
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E68" s="5" t="s">
         <v>277</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="5" t="s">
         <v>281</v>
       </c>
       <c r="F69" s="3" t="s">
@@ -3181,42 +3239,43 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="B67:H67"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B9:H9"/>
     <mergeCell ref="B51:H51"/>
     <mergeCell ref="B55:H55"/>
-    <mergeCell ref="B62:H62"/>
-    <mergeCell ref="B67:H67"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D18"/>
-    <hyperlink r:id="rId2" ref="E18"/>
+    <hyperlink ref="D18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.63"/>
-    <col customWidth="1" min="2" max="2" width="28.63"/>
-    <col customWidth="1" min="3" max="3" width="27.13"/>
-    <col customWidth="1" min="4" max="4" width="24.38"/>
-    <col customWidth="1" min="5" max="5" width="27.13"/>
-    <col customWidth="1" min="6" max="6" width="30.63"/>
-    <col customWidth="1" min="7" max="7" width="28.38"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3242,55 +3301,73 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="13" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>290</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="3" t="s">
         <v>292</v>
@@ -3298,14 +3375,14 @@
       <c r="C7" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3" t="s">
         <v>296</v>
@@ -3313,11 +3390,11 @@
       <c r="E8" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
         <v>299</v>
@@ -3328,38 +3405,38 @@
       <c r="E9" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
         <v>310</v>
@@ -3367,251 +3444,275 @@
       <c r="E12" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="5" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="5" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>321</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>324</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>327</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="5" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>332</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="5" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="13" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>337</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="5" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="5" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="5" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="5" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="5" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="5" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="5" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="5" t="s">
         <v>358</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="5" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>361</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="5" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="33">
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="5" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="5" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="3" t="s">
         <v>371</v>
@@ -3619,143 +3720,155 @@
       <c r="E35" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="5" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>374</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="5" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="5" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="5" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="5" t="s">
         <v>383</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="5" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F40" s="5" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="5" t="s">
         <v>389</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="5" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="5" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="11" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="44">
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="5" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E45" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="5" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E46" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F46" s="5" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="11" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="48">
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="3" t="s">
         <v>406</v>
@@ -3767,45 +3880,57 @@
         <v>408</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="5" t="s">
         <v>410</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E50" s="5" t="s">
         <v>413</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="13" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="52">
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="11" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="53">
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="5" t="s">
         <v>417</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -3821,9 +3946,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -3832,16 +3957,16 @@
       <c r="D54" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E54" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F54" s="5" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="5" t="s">
         <v>426</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -3850,16 +3975,16 @@
       <c r="D55" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E55" s="5" t="s">
         <v>428</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="5" t="s">
         <v>430</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -3868,16 +3993,16 @@
       <c r="D56" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E56" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="F56" s="7" t="s">
+      <c r="F56" s="5" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="5" t="s">
         <v>435</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -3886,14 +4011,14 @@
       <c r="D57" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E57" s="5" t="s">
         <v>437</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="3" t="s">
         <v>439</v>
@@ -3901,19 +4026,19 @@
       <c r="C58" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D58" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E58" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="F58" s="7" t="s">
+      <c r="F58" s="5" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="5" t="s">
         <v>444</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -3922,14 +4047,14 @@
       <c r="D59" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="E59" s="5" t="s">
         <v>447</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="3" t="s">
         <v>449</v>
@@ -3940,14 +4065,14 @@
       <c r="D60" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E60" s="5" t="s">
         <v>451</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="3" t="s">
         <v>453</v>
@@ -3958,14 +4083,14 @@
       <c r="D61" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="E61" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="F61" s="7" t="s">
+      <c r="F61" s="5" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="3" t="s">
         <v>458</v>
@@ -3976,14 +4101,14 @@
       <c r="D62" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E62" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="F62" s="7" t="s">
+      <c r="F62" s="5" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="3" t="s">
         <v>463</v>
@@ -3994,50 +4119,50 @@
       <c r="D63" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E63" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="F63" s="5" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E64" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="5" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="5" t="s">
         <v>473</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E65" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="5" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="3" t="s">
         <v>474</v>
@@ -4048,34 +4173,34 @@
       <c r="D66" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="E66" s="7" t="s">
+      <c r="E66" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="F66" s="7" t="s">
+      <c r="F66" s="5" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="5" t="s">
         <v>467</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="E67" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="F67" s="7" t="s">
+      <c r="F67" s="5" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="5" t="s">
         <v>480</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -4087,13 +4212,13 @@
       <c r="E68" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="F68" s="7" t="s">
+      <c r="F68" s="5" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="5" t="s">
         <v>485</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -4102,14 +4227,14 @@
       <c r="D69" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="F69" s="7" t="s">
+      <c r="F69" s="5" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="3" t="s">
         <v>489</v>
@@ -4120,22 +4245,28 @@
       <c r="D70" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E70" s="5" t="s">
         <v>492</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F70" s="5" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="11" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="72">
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="5" t="s">
         <v>495</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -4144,14 +4275,14 @@
       <c r="D72" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E72" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="F72" s="5" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="3" t="s">
         <v>500</v>
@@ -4159,16 +4290,16 @@
       <c r="C73" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="E73" s="7" t="s">
+      <c r="E73" s="5" t="s">
         <v>502</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="5" t="s">
         <v>504</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -4177,16 +4308,16 @@
       <c r="D74" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="E74" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="F74" s="7" t="s">
+      <c r="F74" s="5" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
-      <c r="B75" s="7" t="s">
+      <c r="B75" s="5" t="s">
         <v>509</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -4195,34 +4326,34 @@
       <c r="D75" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="E75" s="7" t="s">
+      <c r="E75" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="F75" s="7" t="s">
+      <c r="F75" s="5" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="5" t="s">
         <v>512</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="E76" s="7" t="s">
+      <c r="E76" s="5" t="s">
         <v>514</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="5" t="s">
         <v>517</v>
       </c>
       <c r="D77" s="3" t="s">
@@ -4231,50 +4362,56 @@
       <c r="E77" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="F77" s="7" t="s">
+      <c r="F77" s="5" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="5" t="s">
         <v>522</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="E78" s="7" t="s">
+      <c r="E78" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F78" s="7" t="s">
+      <c r="F78" s="5" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
-      <c r="B79" s="12" t="s">
+      <c r="B79" s="11" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="80">
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="5" t="s">
         <v>527</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="E80" s="7" t="s">
+      <c r="E80" s="5" t="s">
         <v>529</v>
       </c>
-      <c r="F80" s="7" t="s">
+      <c r="F80" s="5" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="3" t="s">
         <v>531</v>
@@ -4282,14 +4419,14 @@
       <c r="C81" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="E81" s="7" t="s">
+      <c r="E81" s="5" t="s">
         <v>533</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="3" t="s">
         <v>535</v>
@@ -4303,13 +4440,13 @@
       <c r="E82" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="F82" s="7" t="s">
+      <c r="F82" s="5" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
-      <c r="B83" s="7" t="s">
+      <c r="B83" s="5" t="s">
         <v>540</v>
       </c>
       <c r="C83" s="3" t="s">
@@ -4321,50 +4458,51 @@
       <c r="E83" s="3" t="s">
         <v>543</v>
       </c>
-      <c r="F83" s="7" t="s">
+      <c r="F83" s="5" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
-      <c r="B84" s="12" t="s">
+      <c r="B84" s="11" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="85">
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
     </row>
-    <row r="86">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
     </row>
-    <row r="87">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
     </row>
-    <row r="88">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
     </row>
-    <row r="89">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
     </row>
-    <row r="90">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
     </row>
-    <row r="91">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
     </row>
-    <row r="92">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
     </row>
-    <row r="93">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B51:H51"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B71:H71"/>
     <mergeCell ref="B79:H79"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B2:H2"/>
@@ -4374,7 +4512,12 @@
     <mergeCell ref="B21:H21"/>
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="B71:H71"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>